<commit_message>
Re-did some comet times for consistency
</commit_message>
<xml_diff>
--- a/OpenMP Times - Comet.xlsx
+++ b/OpenMP Times - Comet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Comet" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -562,7 +562,7 @@
                   <c:v>0.98340248962655596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1666666666666667</c:v>
+                  <c:v>1.0220385674931129</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.021505376344086</c:v>
@@ -634,7 +634,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>1.2500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -647,7 +647,7 @@
                   <c:v>1.1975308641975311</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.30508474576271188</c:v>
+                  <c:v>0.98181818181818192</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0042372881355932</c:v>
@@ -747,7 +747,7 @@
                   <c:v>1.1259484066767831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0760517799352751</c:v>
+                  <c:v>1.1545138888888891</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.0008269417626263</c:v>
@@ -816,13 +816,13 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9795918367346941</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="0.000000">
                   <c:v>1.15625</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -835,10 +835,10 @@
                   <c:v>1.021551724137931</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0319888734353269</c:v>
+                  <c:v>1.1815286624203822</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0614525139664805</c:v>
+                  <c:v>1.2036199095022624</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.99627510701350008</c:v>
@@ -907,7 +907,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -919,17 +919,17 @@
                 <c:pt idx="3">
                   <c:v>1.0898876404494382</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0588235294117647</c:v>
+                <c:pt idx="4" formatCode="0.000000">
+                  <c:v>0.80597014925373134</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0128205128205128</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.94402035623409664</c:v>
+                <c:pt idx="6" formatCode="0.000000">
+                  <c:v>1.2428810720268006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0725806451612905</c:v>
+                  <c:v>1.2246777163904237</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.99276105323599373</c:v>
@@ -1484,7 +1484,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1503,7 +1503,7 @@
                   <c:v>0.49170124481327798</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58333333333333337</c:v>
+                  <c:v>0.51101928374655647</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.510752688172043</c:v>
@@ -1575,7 +1575,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>0.31250000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1588,7 +1588,7 @@
                   <c:v>0.29938271604938277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6271186440677971E-2</c:v>
+                  <c:v>0.24545454545454548</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.2510593220338983</c:v>
@@ -1688,7 +1688,7 @@
                   <c:v>0.14074355083459789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13450647249190939</c:v>
+                  <c:v>0.14431423611111113</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.12510336772032829</c:v>
@@ -1757,7 +1757,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1776,10 +1776,10 @@
                   <c:v>8.5129310344827583E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5999072786277234E-2</c:v>
+                  <c:v>9.8460721868365186E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8454376163873374E-2</c:v>
+                  <c:v>0.10030165912518854</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8.302292558445834E-2</c:v>
@@ -1848,7 +1848,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000000">
                   <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1861,16 +1861,16 @@
                   <c:v>6.8117977528089887E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6176470588235295E-2</c:v>
+                  <c:v>5.0373134328358209E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.3301282051282048E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.900127226463104E-2</c:v>
+                  <c:v>7.7680067001675041E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.7036290322580655E-2</c:v>
+                  <c:v>7.6542357274401479E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>6.2047565827249608E-2</c:v>
@@ -8880,8 +8880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8960,7 +8960,7 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="29">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4" s="4">
@@ -8981,7 +8981,7 @@
       <c r="I4" s="4">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="29">
         <v>0.13300000000000001</v>
       </c>
       <c r="K4" s="14">
@@ -8993,7 +8993,7 @@
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="29">
         <v>2E-3</v>
       </c>
       <c r="D5" s="4">
@@ -9002,7 +9002,7 @@
       <c r="E5" s="4">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G5" s="4">
@@ -9012,7 +9012,7 @@
         <v>2.41E-2</v>
       </c>
       <c r="I5" s="4">
-        <v>6.3600000000000004E-2</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="J5" s="4">
         <v>0.13020000000000001</v>
@@ -9038,8 +9038,8 @@
       <c r="F6" s="4">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="G6" s="4">
-        <v>3.5400000000000001E-2</v>
+      <c r="G6" s="29">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H6" s="4">
         <v>2.3599999999999999E-2</v>
@@ -9080,8 +9080,8 @@
       <c r="I7" s="4">
         <v>6.59E-2</v>
       </c>
-      <c r="J7" s="4">
-        <v>0.1236</v>
+      <c r="J7" s="29">
+        <v>0.1152</v>
       </c>
       <c r="K7" s="14">
         <v>4.8371000000000004</v>
@@ -9092,7 +9092,7 @@
       <c r="B8" s="2">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8" s="4">
@@ -9104,17 +9104,17 @@
       <c r="F8" s="4">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H8" s="4">
         <v>2.3199999999999998E-2</v>
       </c>
       <c r="I8" s="4">
-        <v>7.1900000000000006E-2</v>
+        <v>6.2799999999999995E-2</v>
       </c>
       <c r="J8" s="4">
-        <v>0.12529999999999999</v>
+        <v>0.1105</v>
       </c>
       <c r="K8" s="14">
         <v>4.8592000000000004</v>
@@ -9125,7 +9125,7 @@
       <c r="B9" s="16">
         <v>16</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="30">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D9" s="17">
@@ -9138,16 +9138,16 @@
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="G9" s="17">
-        <v>1.0200000000000001E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="H9" s="17">
         <v>2.3400000000000001E-2</v>
       </c>
       <c r="I9" s="17">
-        <v>7.8600000000000003E-2</v>
-      </c>
-      <c r="J9" s="17">
-        <v>0.124</v>
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="J9" s="30">
+        <v>0.1086</v>
       </c>
       <c r="K9" s="18">
         <v>4.8764000000000003</v>
@@ -9259,7 +9259,7 @@
       <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="31">
         <f>C4/C5</f>
         <v>1.5</v>
       </c>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="I15" s="4">
         <f>I4/I5</f>
-        <v>1.1666666666666667</v>
+        <v>1.0220385674931129</v>
       </c>
       <c r="J15" s="4">
         <f>J4/J5</f>
@@ -9301,7 +9301,7 @@
       <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="31">
         <f>C4/C6</f>
         <v>1.2500000000000002</v>
       </c>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="G16" s="4">
         <f>G4/G6</f>
-        <v>0.30508474576271188</v>
+        <v>0.98181818181818192</v>
       </c>
       <c r="H16" s="4">
         <f>H4/H6</f>
@@ -9375,7 +9375,7 @@
       </c>
       <c r="J17" s="4">
         <f>J4/J7</f>
-        <v>1.0760517799352751</v>
+        <v>1.1545138888888891</v>
       </c>
       <c r="K17" s="20">
         <f>K4/K7</f>
@@ -9387,7 +9387,7 @@
       <c r="B18" s="2">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="31">
         <f>C4/C8</f>
         <v>0.6</v>
       </c>
@@ -9395,7 +9395,7 @@
         <f>D4/D8</f>
         <v>1.9795918367346941</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="31">
         <f>E4/E8</f>
         <v>1.15625</v>
       </c>
@@ -9413,11 +9413,11 @@
       </c>
       <c r="I18" s="4">
         <f>I4/I8</f>
-        <v>1.0319888734353269</v>
+        <v>1.1815286624203822</v>
       </c>
       <c r="J18" s="4">
         <f>J4/J8</f>
-        <v>1.0614525139664805</v>
+        <v>1.2036199095022624</v>
       </c>
       <c r="K18" s="20">
         <f>K4/K8</f>
@@ -9429,7 +9429,7 @@
       <c r="B19" s="16">
         <v>16</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="33">
         <f>C4/C9</f>
         <v>1</v>
       </c>
@@ -9445,21 +9445,21 @@
         <f>F4/F9</f>
         <v>1.0898876404494382</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="33">
         <f>G4/G9</f>
-        <v>1.0588235294117647</v>
+        <v>0.80597014925373134</v>
       </c>
       <c r="H19" s="17">
         <f>H4/H9</f>
         <v>1.0128205128205128</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="33">
         <f>I4/I9</f>
-        <v>0.94402035623409664</v>
+        <v>1.2428810720268006</v>
       </c>
       <c r="J19" s="17">
         <f>J4/J9</f>
-        <v>1.0725806451612905</v>
+        <v>1.2246777163904237</v>
       </c>
       <c r="K19" s="18">
         <f>K4/K9</f>
@@ -9568,7 +9568,7 @@
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="31">
         <f>C4/(C5*2)</f>
         <v>0.75</v>
       </c>
@@ -9594,7 +9594,7 @@
       </c>
       <c r="I25" s="4">
         <f>I4/(I5*2)</f>
-        <v>0.58333333333333337</v>
+        <v>0.51101928374655647</v>
       </c>
       <c r="J25" s="4">
         <f>J4/(J5*2)</f>
@@ -9610,7 +9610,7 @@
       <c r="B26" s="2">
         <v>4</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="31">
         <f>C4/(C6*4)</f>
         <v>0.31250000000000006</v>
       </c>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="G26" s="4">
         <f>G4/(G6*4)</f>
-        <v>7.6271186440677971E-2</v>
+        <v>0.24545454545454548</v>
       </c>
       <c r="H26" s="4">
         <f>H4/(H6*4)</f>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="J27" s="4">
         <f>J4/(J7*8)</f>
-        <v>0.13450647249190939</v>
+        <v>0.14431423611111113</v>
       </c>
       <c r="K27" s="20">
         <f>K4/(K7*8)</f>
@@ -9694,7 +9694,7 @@
       <c r="B28" s="2">
         <v>12</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="31">
         <f>C4/(C8*12)</f>
         <v>0.05</v>
       </c>
@@ -9720,11 +9720,11 @@
       </c>
       <c r="I28" s="4">
         <f>I4/(I8*12)</f>
-        <v>8.5999072786277234E-2</v>
+        <v>9.8460721868365186E-2</v>
       </c>
       <c r="J28" s="4">
         <f>J4/(J8*12)</f>
-        <v>8.8454376163873374E-2</v>
+        <v>0.10030165912518854</v>
       </c>
       <c r="K28" s="20">
         <f>K4/(K8*12)</f>
@@ -9736,7 +9736,7 @@
       <c r="B29" s="16">
         <v>16</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="33">
         <f>C4/(C9*16)</f>
         <v>6.25E-2</v>
       </c>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="G29" s="17">
         <f>G4/(G9*16)</f>
-        <v>6.6176470588235295E-2</v>
+        <v>5.0373134328358209E-2</v>
       </c>
       <c r="H29" s="17">
         <f>H4/(H9*16)</f>
@@ -9762,11 +9762,11 @@
       </c>
       <c r="I29" s="17">
         <f>I4/(I9*16)</f>
-        <v>5.900127226463104E-2</v>
+        <v>7.7680067001675041E-2</v>
       </c>
       <c r="J29" s="17">
         <f>J4/(J9*16)</f>
-        <v>6.7036290322580655E-2</v>
+        <v>7.6542357274401479E-2</v>
       </c>
       <c r="K29" s="18">
         <f>K4/(K9*16)</f>
@@ -9794,7 +9794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed MPI Linux graph missing node legend
</commit_message>
<xml_diff>
--- a/OpenMP Times - Comet.xlsx
+++ b/OpenMP Times - Comet.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caponde\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lastw\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82ABFA92-E810-4259-A288-FF941A98534F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27855" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comet" sheetId="1" r:id="rId1"/>
     <sheet name="Linux" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
-  <si>
-    <t>Speedup</t>
-  </si>
-  <si>
-    <t>Efficiency</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Matrix size</t>
   </si>
@@ -39,16 +40,40 @@
     <t>Number of threads</t>
   </si>
   <si>
-    <t>Times</t>
+    <t>Number of nodes</t>
   </si>
   <si>
-    <t>Number of nodes</t>
+    <t>Times - OpenMP (Linux)</t>
+  </si>
+  <si>
+    <t>Speedup - OpenMP (Linux)</t>
+  </si>
+  <si>
+    <t>Efficiency - OpenMP (Linux)</t>
+  </si>
+  <si>
+    <t>Times - MPI (Linux)</t>
+  </si>
+  <si>
+    <t>Speedup - MPI (Linux)</t>
+  </si>
+  <si>
+    <t>Efficiency - MPI (Linux)</t>
+  </si>
+  <si>
+    <t>Times - OpenMP (Comet)</t>
+  </si>
+  <si>
+    <t>Speedup - OpenMP (Comet)</t>
+  </si>
+  <si>
+    <t>Efficiency - OpenMP (Comet)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -254,43 +279,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -303,6 +301,33 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,7 +385,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -944,7 +968,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -995,7 +1018,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1118,7 +1140,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1194,7 +1215,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1301,7 +1321,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1930,7 +1949,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2052,7 +2070,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2128,7 +2145,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2240,7 +2256,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2663,7 +2678,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2785,7 +2799,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2861,7 +2874,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2972,7 +2984,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3399,7 +3410,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3521,7 +3531,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3597,7 +3606,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3709,7 +3717,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4144,7 +4151,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4267,7 +4273,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4343,7 +4348,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4450,7 +4454,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4902,7 +4905,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5024,7 +5026,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5100,7 +5101,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8442,7 +8442,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8472,7 +8478,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8507,7 +8519,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8537,7 +8555,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8567,7 +8591,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8597,7 +8627,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8877,11 +8913,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="A21" sqref="A21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8891,40 +8927,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
+      <c r="A1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="21"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>3</v>
+      <c r="A3" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3">
@@ -8951,16 +8987,16 @@
       <c r="J3" s="3">
         <v>500</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="15">
         <v>6474</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="20">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4" s="4">
@@ -8981,19 +9017,19 @@
       <c r="I4" s="4">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="20">
         <v>0.13300000000000001</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="9">
         <v>4.8411</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="20">
         <v>2E-3</v>
       </c>
       <c r="D5" s="4">
@@ -9002,7 +9038,7 @@
       <c r="E5" s="4">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="20">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G5" s="4">
@@ -9017,12 +9053,12 @@
       <c r="J5" s="4">
         <v>0.13020000000000001</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="9">
         <v>4.8242000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -9038,7 +9074,7 @@
       <c r="F6" s="4">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="20">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="H6" s="4">
@@ -9050,12 +9086,12 @@
       <c r="J6" s="4">
         <v>0.11940000000000001</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="9">
         <v>4.8356000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -9080,19 +9116,19 @@
       <c r="I7" s="4">
         <v>6.59E-2</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="20">
         <v>0.1152</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="9">
         <v>4.8371000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="2">
         <v>12</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="20">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8" s="4">
@@ -9104,7 +9140,7 @@
       <c r="F8" s="4">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="20">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H8" s="4">
@@ -9116,40 +9152,40 @@
       <c r="J8" s="4">
         <v>0.1105</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="9">
         <v>4.8592000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16">
+      <c r="A9" s="29"/>
+      <c r="B9" s="10">
         <v>16</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="21">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="11">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="11">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="11">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="11">
         <v>1.34E-2</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="11">
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="11">
         <v>5.9700000000000003E-2</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="21">
         <v>0.1086</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="12">
         <v>4.8764000000000003</v>
       </c>
       <c r="L9" s="5"/>
@@ -9159,37 +9195,37 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="11"/>
+      <c r="A11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3">
         <v>10</v>
@@ -9215,13 +9251,13 @@
       <c r="J13" s="3">
         <v>500</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="15">
         <v>6474</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>3</v>
+      <c r="A14" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -9250,255 +9286,255 @@
       <c r="J14" s="4">
         <v>1</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C15" s="31">
-        <f>C4/C5</f>
+      <c r="C15" s="22">
+        <f t="shared" ref="C15:K15" si="0">C4/C5</f>
         <v>1.5</v>
       </c>
       <c r="D15" s="4">
-        <f>D4/D5</f>
+        <f t="shared" si="0"/>
         <v>2.1086956521739131</v>
       </c>
       <c r="E15" s="4">
-        <f>E4/E5</f>
+        <f t="shared" si="0"/>
         <v>1.1384615384615386</v>
       </c>
       <c r="F15" s="4">
-        <f>F4/F5</f>
+        <f t="shared" si="0"/>
         <v>1.0777777777777779</v>
       </c>
       <c r="G15" s="4">
-        <f>G4/G5</f>
+        <f t="shared" si="0"/>
         <v>1.0384615384615385</v>
       </c>
       <c r="H15" s="4">
-        <f>H4/H5</f>
+        <f t="shared" si="0"/>
         <v>0.98340248962655596</v>
       </c>
       <c r="I15" s="4">
-        <f>I4/I5</f>
+        <f t="shared" si="0"/>
         <v>1.0220385674931129</v>
       </c>
       <c r="J15" s="4">
-        <f>J4/J5</f>
+        <f t="shared" si="0"/>
         <v>1.021505376344086</v>
       </c>
-      <c r="K15" s="20">
-        <f>K4/K5</f>
+      <c r="K15" s="14">
+        <f t="shared" si="0"/>
         <v>1.0035031715103022</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C16" s="31">
-        <f>C4/C6</f>
+      <c r="C16" s="22">
+        <f t="shared" ref="C16:K16" si="1">C4/C6</f>
         <v>1.2500000000000002</v>
       </c>
       <c r="D16" s="4">
-        <f>D4/D6</f>
+        <f t="shared" si="1"/>
         <v>1.7962962962962963</v>
       </c>
       <c r="E16" s="4">
-        <f>E4/E6</f>
+        <f t="shared" si="1"/>
         <v>1.0136986301369864</v>
       </c>
       <c r="F16" s="4">
-        <f>F4/F6</f>
+        <f t="shared" si="1"/>
         <v>1.1975308641975311</v>
       </c>
       <c r="G16" s="4">
-        <f>G4/G6</f>
+        <f t="shared" si="1"/>
         <v>0.98181818181818192</v>
       </c>
       <c r="H16" s="4">
-        <f>H4/H6</f>
+        <f t="shared" si="1"/>
         <v>1.0042372881355932</v>
       </c>
       <c r="I16" s="4">
-        <f>I4/I6</f>
+        <f t="shared" si="1"/>
         <v>1.0816326530612246</v>
       </c>
       <c r="J16" s="4">
-        <f>J4/J6</f>
+        <f t="shared" si="1"/>
         <v>1.1139028475711892</v>
       </c>
-      <c r="K16" s="20">
-        <f>K4/K6</f>
+      <c r="K16" s="14">
+        <f t="shared" si="1"/>
         <v>1.0011373976342128</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="2">
         <v>8</v>
       </c>
       <c r="C17" s="4">
-        <f>C4/C7</f>
+        <f t="shared" ref="C17:K17" si="2">C4/C7</f>
         <v>1.4285714285714286</v>
       </c>
       <c r="D17" s="4">
-        <f>D4/D7</f>
+        <f t="shared" si="2"/>
         <v>1.2933333333333334</v>
       </c>
       <c r="E17" s="4">
-        <f>E4/E7</f>
+        <f t="shared" si="2"/>
         <v>1.1935483870967742</v>
       </c>
       <c r="F17" s="4">
-        <f>F4/F7</f>
+        <f t="shared" si="2"/>
         <v>1.1022727272727273</v>
       </c>
       <c r="G17" s="4">
-        <f>G4/G7</f>
+        <f t="shared" si="2"/>
         <v>0.90756302521008403</v>
       </c>
       <c r="H17" s="4">
-        <f>H4/H7</f>
+        <f t="shared" si="2"/>
         <v>0.92217898832684819</v>
       </c>
       <c r="I17" s="4">
-        <f>I4/I7</f>
+        <f t="shared" si="2"/>
         <v>1.1259484066767831</v>
       </c>
       <c r="J17" s="4">
-        <f>J4/J7</f>
+        <f t="shared" si="2"/>
         <v>1.1545138888888891</v>
       </c>
-      <c r="K17" s="20">
-        <f>K4/K7</f>
+      <c r="K17" s="14">
+        <f t="shared" si="2"/>
         <v>1.0008269417626263</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="2">
         <v>12</v>
       </c>
-      <c r="C18" s="31">
-        <f>C4/C8</f>
+      <c r="C18" s="22">
+        <f t="shared" ref="C18:K18" si="3">C4/C8</f>
         <v>0.6</v>
       </c>
       <c r="D18" s="4">
-        <f>D4/D8</f>
+        <f t="shared" si="3"/>
         <v>1.9795918367346941</v>
       </c>
-      <c r="E18" s="31">
-        <f>E4/E8</f>
+      <c r="E18" s="22">
+        <f t="shared" si="3"/>
         <v>1.15625</v>
       </c>
       <c r="F18" s="4">
-        <f>F4/F8</f>
+        <f t="shared" si="3"/>
         <v>1.0898876404494382</v>
       </c>
       <c r="G18" s="4">
-        <f>G4/G8</f>
+        <f t="shared" si="3"/>
         <v>0.83076923076923082</v>
       </c>
       <c r="H18" s="4">
-        <f>H4/H8</f>
+        <f t="shared" si="3"/>
         <v>1.021551724137931</v>
       </c>
       <c r="I18" s="4">
-        <f>I4/I8</f>
+        <f t="shared" si="3"/>
         <v>1.1815286624203822</v>
       </c>
       <c r="J18" s="4">
-        <f>J4/J8</f>
+        <f t="shared" si="3"/>
         <v>1.2036199095022624</v>
       </c>
-      <c r="K18" s="20">
-        <f>K4/K8</f>
+      <c r="K18" s="14">
+        <f t="shared" si="3"/>
         <v>0.99627510701350008</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16">
+      <c r="A19" s="29"/>
+      <c r="B19" s="10">
         <v>16</v>
       </c>
-      <c r="C19" s="33">
-        <f>C4/C9</f>
+      <c r="C19" s="24">
+        <f t="shared" ref="C19:K19" si="4">C4/C9</f>
         <v>1</v>
       </c>
-      <c r="D19" s="17">
-        <f>D4/D9</f>
+      <c r="D19" s="11">
+        <f t="shared" si="4"/>
         <v>2.0208333333333335</v>
       </c>
-      <c r="E19" s="17">
-        <f>E4/E9</f>
+      <c r="E19" s="11">
+        <f t="shared" si="4"/>
         <v>1.1384615384615386</v>
       </c>
-      <c r="F19" s="17">
-        <f>F4/F9</f>
+      <c r="F19" s="11">
+        <f t="shared" si="4"/>
         <v>1.0898876404494382</v>
       </c>
-      <c r="G19" s="33">
-        <f>G4/G9</f>
+      <c r="G19" s="24">
+        <f t="shared" si="4"/>
         <v>0.80597014925373134</v>
       </c>
-      <c r="H19" s="17">
-        <f>H4/H9</f>
+      <c r="H19" s="11">
+        <f t="shared" si="4"/>
         <v>1.0128205128205128</v>
       </c>
-      <c r="I19" s="33">
-        <f>I4/I9</f>
+      <c r="I19" s="24">
+        <f t="shared" si="4"/>
         <v>1.2428810720268006</v>
       </c>
-      <c r="J19" s="17">
-        <f>J4/J9</f>
+      <c r="J19" s="11">
+        <f t="shared" si="4"/>
         <v>1.2246777163904237</v>
       </c>
-      <c r="K19" s="18">
-        <f>K4/K9</f>
+      <c r="K19" s="12">
+        <f t="shared" si="4"/>
         <v>0.99276105323599373</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="11"/>
+      <c r="A21" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="21"/>
+      <c r="C22" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3">
         <v>10</v>
@@ -9524,13 +9560,13 @@
       <c r="J23" s="3">
         <v>500</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="16">
         <v>6474</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>3</v>
+      <c r="A24" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -9541,249 +9577,249 @@
       <c r="D24" s="4">
         <v>1</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>1</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>1</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>1</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>1</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="6">
         <v>1</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="31">
-        <f>C4/(C5*2)</f>
+      <c r="C25" s="22">
+        <f t="shared" ref="C25:K25" si="5">C4/(C5*2)</f>
         <v>0.75</v>
       </c>
       <c r="D25" s="4">
-        <f>D4/(D5*2)</f>
+        <f t="shared" si="5"/>
         <v>1.0543478260869565</v>
       </c>
       <c r="E25" s="4">
-        <f>E4/(E5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.56923076923076932</v>
       </c>
       <c r="F25" s="4">
-        <f>F4/(F5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.53888888888888897</v>
       </c>
       <c r="G25" s="4">
-        <f>G4/(G5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.51923076923076927</v>
       </c>
       <c r="H25" s="4">
-        <f>H4/(H5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.49170124481327798</v>
       </c>
       <c r="I25" s="4">
-        <f>I4/(I5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.51101928374655647</v>
       </c>
       <c r="J25" s="4">
-        <f>J4/(J5*2)</f>
+        <f t="shared" si="5"/>
         <v>0.510752688172043</v>
       </c>
-      <c r="K25" s="20">
-        <f>K4/(K5*2)</f>
+      <c r="K25" s="14">
+        <f t="shared" si="5"/>
         <v>0.50175158575515111</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="2">
         <v>4</v>
       </c>
-      <c r="C26" s="31">
-        <f>C4/(C6*4)</f>
+      <c r="C26" s="22">
+        <f t="shared" ref="C26:K26" si="6">C4/(C6*4)</f>
         <v>0.31250000000000006</v>
       </c>
       <c r="D26" s="4">
-        <f>D4/(D6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.44907407407407407</v>
       </c>
       <c r="E26" s="4">
-        <f>E4/(E6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.25342465753424659</v>
       </c>
       <c r="F26" s="4">
-        <f>F4/(F6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.29938271604938277</v>
       </c>
       <c r="G26" s="4">
-        <f>G4/(G6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.24545454545454548</v>
       </c>
       <c r="H26" s="4">
-        <f>H4/(H6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.2510593220338983</v>
       </c>
       <c r="I26" s="4">
-        <f>I4/(I6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.27040816326530615</v>
       </c>
       <c r="J26" s="4">
-        <f>J4/(J6*4)</f>
+        <f t="shared" si="6"/>
         <v>0.2784757118927973</v>
       </c>
-      <c r="K26" s="20">
-        <f>K4/(K6*4)</f>
+      <c r="K26" s="14">
+        <f t="shared" si="6"/>
         <v>0.25028434940855321</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="2">
         <v>8</v>
       </c>
       <c r="C27" s="4">
-        <f>C4/(C7*8)</f>
+        <f t="shared" ref="C27:K27" si="7">C4/(C7*8)</f>
         <v>0.17857142857142858</v>
       </c>
       <c r="D27" s="4">
-        <f>D4/(D7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.16166666666666668</v>
       </c>
       <c r="E27" s="4">
-        <f>E4/(E7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.14919354838709678</v>
       </c>
       <c r="F27" s="4">
-        <f>F4/(F7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.13778409090909091</v>
       </c>
       <c r="G27" s="4">
-        <f>G4/(G7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.1134453781512605</v>
       </c>
       <c r="H27" s="4">
-        <f>H4/(H7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.11527237354085602</v>
       </c>
       <c r="I27" s="4">
-        <f>I4/(I7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.14074355083459789</v>
       </c>
       <c r="J27" s="4">
-        <f>J4/(J7*8)</f>
+        <f t="shared" si="7"/>
         <v>0.14431423611111113</v>
       </c>
-      <c r="K27" s="20">
-        <f>K4/(K7*8)</f>
+      <c r="K27" s="14">
+        <f t="shared" si="7"/>
         <v>0.12510336772032829</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="2">
         <v>12</v>
       </c>
-      <c r="C28" s="31">
-        <f>C4/(C8*12)</f>
+      <c r="C28" s="22">
+        <f t="shared" ref="C28:K28" si="8">C4/(C8*12)</f>
         <v>0.05</v>
       </c>
       <c r="D28" s="4">
-        <f>D4/(D8*12)</f>
+        <f t="shared" si="8"/>
         <v>0.16496598639455784</v>
       </c>
       <c r="E28" s="4">
-        <f>E4/(E8*12)</f>
+        <f t="shared" si="8"/>
         <v>9.6354166666666657E-2</v>
       </c>
       <c r="F28" s="4">
-        <f>F4/(F8*12)</f>
+        <f t="shared" si="8"/>
         <v>9.0823970037453183E-2</v>
       </c>
       <c r="G28" s="4">
-        <f>G4/(G8*12)</f>
+        <f t="shared" si="8"/>
         <v>6.9230769230769235E-2</v>
       </c>
       <c r="H28" s="4">
-        <f>H4/(H8*12)</f>
+        <f t="shared" si="8"/>
         <v>8.5129310344827583E-2</v>
       </c>
       <c r="I28" s="4">
-        <f>I4/(I8*12)</f>
+        <f t="shared" si="8"/>
         <v>9.8460721868365186E-2</v>
       </c>
       <c r="J28" s="4">
-        <f>J4/(J8*12)</f>
+        <f t="shared" si="8"/>
         <v>0.10030165912518854</v>
       </c>
-      <c r="K28" s="20">
-        <f>K4/(K8*12)</f>
+      <c r="K28" s="14">
+        <f t="shared" si="8"/>
         <v>8.302292558445834E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16">
+      <c r="A29" s="29"/>
+      <c r="B29" s="10">
         <v>16</v>
       </c>
-      <c r="C29" s="33">
-        <f>C4/(C9*16)</f>
+      <c r="C29" s="24">
+        <f t="shared" ref="C29:K29" si="9">C4/(C9*16)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D29" s="17">
-        <f>D4/(D9*16)</f>
+      <c r="D29" s="11">
+        <f t="shared" si="9"/>
         <v>0.12630208333333334</v>
       </c>
-      <c r="E29" s="17">
-        <f>E4/(E9*16)</f>
+      <c r="E29" s="11">
+        <f t="shared" si="9"/>
         <v>7.1153846153846165E-2</v>
       </c>
-      <c r="F29" s="17">
-        <f>F4/(F9*16)</f>
+      <c r="F29" s="11">
+        <f t="shared" si="9"/>
         <v>6.8117977528089887E-2</v>
       </c>
-      <c r="G29" s="17">
-        <f>G4/(G9*16)</f>
+      <c r="G29" s="11">
+        <f t="shared" si="9"/>
         <v>5.0373134328358209E-2</v>
       </c>
-      <c r="H29" s="17">
-        <f>H4/(H9*16)</f>
+      <c r="H29" s="11">
+        <f t="shared" si="9"/>
         <v>6.3301282051282048E-2</v>
       </c>
-      <c r="I29" s="17">
-        <f>I4/(I9*16)</f>
+      <c r="I29" s="11">
+        <f t="shared" si="9"/>
         <v>7.7680067001675041E-2</v>
       </c>
-      <c r="J29" s="17">
-        <f>J4/(J9*16)</f>
+      <c r="J29" s="11">
+        <f t="shared" si="9"/>
         <v>7.6542357274401479E-2</v>
       </c>
-      <c r="K29" s="18">
-        <f>K4/(K9*16)</f>
+      <c r="K29" s="12">
+        <f t="shared" si="9"/>
         <v>6.2047565827249608E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="C22:K22"/>
     <mergeCell ref="A24:A29"/>
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9791,45 +9827,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26"/>
-      <c r="B1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="21"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
         <v>10</v>
@@ -9852,13 +9888,13 @@
       <c r="I3" s="4">
         <v>300</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>3</v>
+      <c r="A4" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -9884,12 +9920,12 @@
       <c r="I4" s="3">
         <v>0.18060000000000001</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="16">
         <v>0.29070000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -9914,16 +9950,16 @@
       <c r="I5" s="4">
         <v>0.1623</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="14">
         <v>0.25659999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="19">
         <v>1.6400000000000001E-2</v>
       </c>
       <c r="D6" s="4">
@@ -9941,74 +9977,74 @@
       <c r="H6" s="4">
         <v>5.4699999999999999E-2</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="20">
         <v>0.1404</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="14">
         <v>0.23960000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="17">
+      <c r="A7" s="29"/>
+      <c r="B7" s="11">
         <v>8</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="10">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="11">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="11">
         <v>2.7900000000000001E-2</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="21">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="21">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="11">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="11">
         <v>0.13739999999999999</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="12">
         <v>0.23630000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
+      <c r="A9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="21"/>
+      <c r="C10" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
         <v>10</v>
@@ -10031,13 +10067,13 @@
       <c r="I11" s="4">
         <v>300</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>3</v>
+      <c r="A12" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -10063,155 +10099,155 @@
       <c r="I12" s="3">
         <v>1</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="4">
         <v>2</v>
       </c>
       <c r="C13" s="2">
-        <f>C4/C5</f>
+        <f t="shared" ref="C13:J13" si="0">C4/C5</f>
         <v>1.0538922155688624</v>
       </c>
       <c r="D13" s="4">
-        <f>D4/D5</f>
+        <f t="shared" si="0"/>
         <v>1.0377358490566038</v>
       </c>
       <c r="E13" s="4">
-        <f>E4/E5</f>
+        <f t="shared" si="0"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="F13" s="4">
-        <f>F4/F5</f>
+        <f t="shared" si="0"/>
         <v>0.92181069958847739</v>
       </c>
       <c r="G13" s="4">
-        <f>G4/G5</f>
+        <f t="shared" si="0"/>
         <v>0.82933333333333337</v>
       </c>
       <c r="H13" s="4">
-        <f>H4/H5</f>
+        <f t="shared" si="0"/>
         <v>1.0137693631669535</v>
       </c>
       <c r="I13" s="4">
-        <f>I4/I5</f>
+        <f t="shared" si="0"/>
         <v>1.1127541589648799</v>
       </c>
-      <c r="J13" s="34">
-        <f>J4/J5</f>
+      <c r="J13" s="25">
+        <f t="shared" si="0"/>
         <v>1.1328916601714731</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="4">
         <v>4</v>
       </c>
-      <c r="C14" s="32">
-        <f>C4/C6</f>
+      <c r="C14" s="23">
+        <f t="shared" ref="C14:J14" si="1">C4/C6</f>
         <v>1.0731707317073171</v>
       </c>
-      <c r="D14" s="31">
-        <f>D4/D6</f>
+      <c r="D14" s="22">
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="E14" s="31">
-        <f>E4/E6</f>
+      <c r="E14" s="22">
+        <f t="shared" si="1"/>
         <v>0.90804597701149414</v>
       </c>
-      <c r="F14" s="31">
-        <f>F4/F6</f>
+      <c r="F14" s="22">
+        <f t="shared" si="1"/>
         <v>0.84848484848484851</v>
       </c>
-      <c r="G14" s="31">
-        <f>G4/G6</f>
+      <c r="G14" s="22">
+        <f t="shared" si="1"/>
         <v>0.852054794520548</v>
       </c>
-      <c r="H14" s="31">
-        <f>H4/H6</f>
+      <c r="H14" s="22">
+        <f t="shared" si="1"/>
         <v>1.076782449725777</v>
       </c>
-      <c r="I14" s="31">
-        <f>I4/I6</f>
+      <c r="I14" s="22">
+        <f t="shared" si="1"/>
         <v>1.2863247863247864</v>
       </c>
-      <c r="J14" s="34">
-        <f>J4/J6</f>
+      <c r="J14" s="25">
+        <f t="shared" si="1"/>
         <v>1.2132721202003338</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="17">
+      <c r="A15" s="29"/>
+      <c r="B15" s="11">
         <v>8</v>
       </c>
-      <c r="C15" s="16">
-        <f>C4/C7</f>
+      <c r="C15" s="10">
+        <f t="shared" ref="C15:J15" si="2">C4/C7</f>
         <v>1.1139240506329113</v>
       </c>
-      <c r="D15" s="17">
-        <f>D4/D7</f>
+      <c r="D15" s="11">
+        <f t="shared" si="2"/>
         <v>1.807511737089202</v>
       </c>
-      <c r="E15" s="17">
-        <f>E4/E7</f>
+      <c r="E15" s="11">
+        <f t="shared" si="2"/>
         <v>0.84946236559139776</v>
       </c>
-      <c r="F15" s="33">
-        <f>F4/F7</f>
+      <c r="F15" s="24">
+        <f t="shared" si="2"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="G15" s="17">
-        <f>G4/G7</f>
+      <c r="G15" s="11">
+        <f t="shared" si="2"/>
         <v>0.84054054054054061</v>
       </c>
-      <c r="H15" s="17">
-        <f>H4/H7</f>
+      <c r="H15" s="11">
+        <f t="shared" si="2"/>
         <v>1.1971544715447155</v>
       </c>
-      <c r="I15" s="17">
-        <f>I4/I7</f>
+      <c r="I15" s="11">
+        <f t="shared" si="2"/>
         <v>1.314410480349345</v>
       </c>
-      <c r="J15" s="18">
-        <f>J4/J7</f>
+      <c r="J15" s="12">
+        <f t="shared" si="2"/>
         <v>1.2302158273381294</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
+      <c r="A17" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="21"/>
+      <c r="C18" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
         <v>10</v>
@@ -10234,13 +10270,13 @@
       <c r="I19" s="4">
         <v>300</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>3</v>
+      <c r="A20" s="28" t="s">
+        <v>1</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -10266,177 +10302,177 @@
       <c r="I20" s="3">
         <v>1</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="4">
         <v>2</v>
       </c>
       <c r="C21" s="2">
-        <f>C4/(C5*2)</f>
+        <f t="shared" ref="C21:J21" si="3">C4/(C5*2)</f>
         <v>0.52694610778443118</v>
       </c>
       <c r="D21" s="4">
-        <f>D4/(D5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.51886792452830188</v>
       </c>
       <c r="E21" s="4">
-        <f>E4/(E5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.4575289575289575</v>
       </c>
       <c r="F21" s="4">
-        <f>F4/(F5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.46090534979423869</v>
       </c>
       <c r="G21" s="4">
-        <f>G4/(G5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.41466666666666668</v>
       </c>
       <c r="H21" s="4">
-        <f>H4/(H5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.50688468158347677</v>
       </c>
       <c r="I21" s="4">
-        <f>I4/(I5*2)</f>
+        <f t="shared" si="3"/>
         <v>0.55637707948243997</v>
       </c>
-      <c r="J21" s="20">
-        <f>J4/(J5*2)</f>
+      <c r="J21" s="14">
+        <f t="shared" si="3"/>
         <v>0.56644583008573657</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="4">
         <v>4</v>
       </c>
-      <c r="C22" s="32">
-        <f>C4/(C6*4)</f>
+      <c r="C22" s="23">
+        <f t="shared" ref="C22:J22" si="4">C4/(C6*4)</f>
         <v>0.26829268292682928</v>
       </c>
-      <c r="D22" s="31">
-        <f>D4/(D6*4)</f>
+      <c r="D22" s="22">
+        <f t="shared" si="4"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="E22" s="31">
-        <f>E4/(E6*4)</f>
+      <c r="E22" s="22">
+        <f t="shared" si="4"/>
         <v>0.22701149425287354</v>
       </c>
-      <c r="F22" s="31">
-        <f>F4/(F6*4)</f>
+      <c r="F22" s="22">
+        <f t="shared" si="4"/>
         <v>0.21212121212121213</v>
       </c>
-      <c r="G22" s="31">
-        <f>G4/(G6*4)</f>
+      <c r="G22" s="22">
+        <f t="shared" si="4"/>
         <v>0.213013698630137</v>
       </c>
-      <c r="H22" s="31">
-        <f>H4/(H6*4)</f>
+      <c r="H22" s="22">
+        <f t="shared" si="4"/>
         <v>0.26919561243144424</v>
       </c>
-      <c r="I22" s="31">
-        <f>I4/(I6*4)</f>
+      <c r="I22" s="22">
+        <f t="shared" si="4"/>
         <v>0.3215811965811966</v>
       </c>
-      <c r="J22" s="34">
-        <f>J4/(J6*4)</f>
+      <c r="J22" s="25">
+        <f t="shared" si="4"/>
         <v>0.30331803005008345</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="17">
+      <c r="A23" s="29"/>
+      <c r="B23" s="11">
         <v>8</v>
       </c>
-      <c r="C23" s="16">
-        <f>C4/(C7*8)</f>
+      <c r="C23" s="10">
+        <f t="shared" ref="C23:J23" si="5">C4/(C7*8)</f>
         <v>0.13924050632911392</v>
       </c>
-      <c r="D23" s="17">
-        <f>D4/(D7*8)</f>
+      <c r="D23" s="11">
+        <f t="shared" si="5"/>
         <v>0.22593896713615025</v>
       </c>
-      <c r="E23" s="17">
-        <f>E4/(E7*8)</f>
+      <c r="E23" s="11">
+        <f t="shared" si="5"/>
         <v>0.10618279569892472</v>
       </c>
-      <c r="F23" s="33">
-        <f>F4/(F7*8)</f>
+      <c r="F23" s="24">
+        <f t="shared" si="5"/>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="G23" s="17">
-        <f>G4/(G7*8)</f>
+      <c r="G23" s="11">
+        <f t="shared" si="5"/>
         <v>0.10506756756756758</v>
       </c>
-      <c r="H23" s="17">
-        <f>H4/(H7*8)</f>
+      <c r="H23" s="11">
+        <f t="shared" si="5"/>
         <v>0.14964430894308944</v>
       </c>
-      <c r="I23" s="17">
-        <f>I4/(I7*8)</f>
+      <c r="I23" s="11">
+        <f t="shared" si="5"/>
         <v>0.16430131004366813</v>
       </c>
-      <c r="J23" s="18">
-        <f>J4/(J7*8)</f>
+      <c r="J23" s="12">
+        <f t="shared" si="5"/>
         <v>0.15377697841726617</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="19"/>
+      <c r="A33" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="20"/>
+      <c r="C34" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3">
         <v>10</v>
@@ -10462,13 +10498,13 @@
       <c r="J35" s="3">
         <v>500</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="16">
         <v>6474</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>5</v>
+      <c r="A36" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
@@ -10497,12 +10533,12 @@
       <c r="J36" s="4">
         <v>1.5349999999999999E-3</v>
       </c>
-      <c r="K36" s="20">
+      <c r="K36" s="14">
         <v>0.27806399999999998</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="2">
         <v>2</v>
       </c>
@@ -10512,127 +10548,127 @@
       <c r="D37" s="4">
         <v>9.1000000000000003E-5</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>2.5900000000000001E-4</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>1.08E-4</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>1.1900000000000001E-4</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="6">
         <v>1.3100000000000001E-4</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="6">
         <v>6.8599999999999998E-4</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="6">
         <v>1.413E-3</v>
       </c>
-      <c r="K37" s="20">
+      <c r="K37" s="14">
         <v>0.14058499999999999</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="2">
         <v>4</v>
       </c>
       <c r="C38" s="4">
         <v>2.0599999999999999E-4</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>2.1699999999999999E-4</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>1.54E-4</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>2.5799999999999998E-4</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <v>3.0899999999999998E-4</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="6">
         <v>2.1499999999999999E-4</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="6">
         <v>7.18E-4</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="6">
         <v>1.0709999999999999E-3</v>
       </c>
-      <c r="K38" s="20">
+      <c r="K38" s="14">
         <v>8.8022000000000003E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16">
+      <c r="A39" s="29"/>
+      <c r="B39" s="10">
         <v>8</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="11">
         <v>3.5300000000000002E-4</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="11">
         <v>4.1199999999999999E-4</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="11">
         <v>5.4500000000000002E-4</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="11">
         <v>4.4299999999999998E-4</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="11">
         <v>3.3399999999999999E-4</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H39" s="11">
         <v>4.4499999999999997E-4</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="11">
         <v>1.067E-3</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="11">
         <v>1.426E-3</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="12">
         <v>5.2038000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="11"/>
+      <c r="A41" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="32"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="21"/>
+      <c r="C42" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="36"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3">
         <v>10</v>
@@ -10658,13 +10694,13 @@
       <c r="J43" s="3">
         <v>500</v>
       </c>
-      <c r="K43" s="25">
+      <c r="K43" s="16">
         <v>6474</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>5</v>
+      <c r="A44" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
@@ -10675,187 +10711,187 @@
       <c r="D44" s="4">
         <v>1</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="6">
         <v>1</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="6">
         <v>1</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="6">
         <v>1</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="6">
         <v>1</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="6">
         <v>1</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="6">
         <v>1</v>
       </c>
-      <c r="K44" s="20">
+      <c r="K44" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="2">
         <v>2</v>
       </c>
       <c r="C45" s="4">
-        <f>C36/C37</f>
+        <f t="shared" ref="C45:K45" si="6">C36/C37</f>
         <v>0.12941176470588234</v>
       </c>
       <c r="D45" s="4">
-        <f>D36/D37</f>
+        <f t="shared" si="6"/>
         <v>0.23076923076923075</v>
       </c>
       <c r="E45" s="4">
-        <f>E36/E37</f>
+        <f t="shared" si="6"/>
         <v>0.12355212355212354</v>
       </c>
       <c r="F45" s="4">
-        <f>F36/F37</f>
+        <f t="shared" si="6"/>
         <v>0.20370370370370369</v>
       </c>
       <c r="G45" s="4">
-        <f>G36/G37</f>
+        <f t="shared" si="6"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="H45" s="4">
-        <f>H36/H37</f>
+        <f t="shared" si="6"/>
         <v>0.22900763358778625</v>
       </c>
       <c r="I45" s="4">
-        <f>I36/I37</f>
+        <f t="shared" si="6"/>
         <v>0.81049562682215737</v>
       </c>
       <c r="J45" s="4">
-        <f>J36/J37</f>
+        <f t="shared" si="6"/>
         <v>1.0863411181882519</v>
       </c>
-      <c r="K45" s="20">
-        <f>K36/K37</f>
+      <c r="K45" s="14">
+        <f t="shared" si="6"/>
         <v>1.9779066045452929</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="2">
         <v>4</v>
       </c>
       <c r="C46" s="4">
-        <f>C36/C38</f>
+        <f t="shared" ref="C46:K46" si="7">C36/C38</f>
         <v>5.3398058252427182E-2</v>
       </c>
       <c r="D46" s="4">
-        <f>D36/D38</f>
+        <f t="shared" si="7"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="E46" s="4">
-        <f>E36/E38</f>
+        <f t="shared" si="7"/>
         <v>0.20779220779220778</v>
       </c>
       <c r="F46" s="4">
-        <f>F36/F38</f>
+        <f t="shared" si="7"/>
         <v>8.5271317829457363E-2</v>
       </c>
       <c r="G46" s="4">
-        <f>G36/G38</f>
+        <f t="shared" si="7"/>
         <v>9.0614886731391592E-2</v>
       </c>
       <c r="H46" s="4">
-        <f>H36/H38</f>
+        <f t="shared" si="7"/>
         <v>0.13953488372093023</v>
       </c>
       <c r="I46" s="4">
-        <f>I36/I38</f>
+        <f t="shared" si="7"/>
         <v>0.77437325905292476</v>
       </c>
-      <c r="J46" s="31">
-        <f>J36/J38</f>
+      <c r="J46" s="22">
+        <f t="shared" si="7"/>
         <v>1.4332399626517274</v>
       </c>
-      <c r="K46" s="20">
-        <f>K36/K38</f>
+      <c r="K46" s="14">
+        <f t="shared" si="7"/>
         <v>3.1590284247120035</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-      <c r="B47" s="16">
+      <c r="A47" s="29"/>
+      <c r="B47" s="10">
         <v>8</v>
       </c>
-      <c r="C47" s="17">
-        <f>C36/C39</f>
+      <c r="C47" s="11">
+        <f t="shared" ref="C47:K47" si="8">C36/C39</f>
         <v>3.1161473087818695E-2</v>
       </c>
-      <c r="D47" s="17">
-        <f>D36/D39</f>
+      <c r="D47" s="11">
+        <f t="shared" si="8"/>
         <v>5.0970873786407765E-2</v>
       </c>
-      <c r="E47" s="17">
-        <f>E36/E39</f>
+      <c r="E47" s="11">
+        <f t="shared" si="8"/>
         <v>5.8715596330275226E-2</v>
       </c>
-      <c r="F47" s="17">
-        <f>F36/F39</f>
+      <c r="F47" s="11">
+        <f t="shared" si="8"/>
         <v>4.9661399548532735E-2</v>
       </c>
-      <c r="G47" s="17">
-        <f>G36/G39</f>
+      <c r="G47" s="11">
+        <f t="shared" si="8"/>
         <v>8.3832335329341326E-2</v>
       </c>
-      <c r="H47" s="17">
-        <f>H36/H39</f>
+      <c r="H47" s="11">
+        <f t="shared" si="8"/>
         <v>6.7415730337078664E-2</v>
       </c>
-      <c r="I47" s="17">
-        <f>I36/I39</f>
+      <c r="I47" s="11">
+        <f t="shared" si="8"/>
         <v>0.52108716026241797</v>
       </c>
-      <c r="J47" s="17">
-        <f>J36/J39</f>
+      <c r="J47" s="11">
+        <f t="shared" si="8"/>
         <v>1.0764375876577841</v>
       </c>
-      <c r="K47" s="36">
-        <f>K36/K39</f>
+      <c r="K47" s="27">
+        <f t="shared" si="8"/>
         <v>5.3434797647872703</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="11"/>
+      <c r="A49" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="21"/>
+      <c r="C50" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="1"/>
       <c r="C51" s="3">
         <v>10</v>
@@ -10881,13 +10917,13 @@
       <c r="J51" s="3">
         <v>500</v>
       </c>
-      <c r="K51" s="25">
+      <c r="K51" s="16">
         <v>6474</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>5</v>
+      <c r="A52" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="B52" s="2">
         <v>1</v>
@@ -10898,156 +10934,167 @@
       <c r="D52" s="4">
         <v>1</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="6">
         <v>1</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="6">
         <v>1</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="6">
         <v>1</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="6">
         <v>1</v>
       </c>
-      <c r="I52" s="7">
+      <c r="I52" s="6">
         <v>1</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="6">
         <v>1</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K52" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="2">
         <v>2</v>
       </c>
       <c r="C53" s="4">
-        <f>C36/(C37*2)</f>
+        <f t="shared" ref="C53:K53" si="9">C36/(C37*2)</f>
         <v>6.4705882352941169E-2</v>
       </c>
       <c r="D53" s="4">
-        <f>D36/(D37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.11538461538461538</v>
       </c>
       <c r="E53" s="4">
-        <f>E36/(E37*2)</f>
+        <f t="shared" si="9"/>
         <v>6.1776061776061771E-2</v>
       </c>
       <c r="F53" s="4">
-        <f>F36/(F37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.10185185185185185</v>
       </c>
       <c r="G53" s="4">
-        <f>G36/(G37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="H53" s="4">
-        <f>H36/(H37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.11450381679389313</v>
       </c>
       <c r="I53" s="4">
-        <f>I36/(I37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.40524781341107868</v>
       </c>
       <c r="J53" s="4">
-        <f>J36/(J37*2)</f>
+        <f t="shared" si="9"/>
         <v>0.54317055909412593</v>
       </c>
-      <c r="K53" s="20">
-        <f>K36/(K37*2)</f>
+      <c r="K53" s="14">
+        <f t="shared" si="9"/>
         <v>0.98895330227264644</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="28"/>
       <c r="B54" s="2">
         <v>4</v>
       </c>
-      <c r="C54" s="31">
-        <f>C36/(C38*4)</f>
+      <c r="C54" s="22">
+        <f t="shared" ref="C54:K54" si="10">C36/(C38*4)</f>
         <v>1.3349514563106795E-2</v>
       </c>
-      <c r="D54" s="31">
-        <f>D36/(D38*4)</f>
+      <c r="D54" s="22">
+        <f t="shared" si="10"/>
         <v>2.4193548387096774E-2</v>
       </c>
-      <c r="E54" s="31">
-        <f>E36/(E38*4)</f>
+      <c r="E54" s="22">
+        <f t="shared" si="10"/>
         <v>5.1948051948051945E-2</v>
       </c>
-      <c r="F54" s="31">
-        <f>F36/(F38*4)</f>
+      <c r="F54" s="22">
+        <f t="shared" si="10"/>
         <v>2.1317829457364341E-2</v>
       </c>
-      <c r="G54" s="31">
-        <f>G36/(G38*4)</f>
+      <c r="G54" s="22">
+        <f t="shared" si="10"/>
         <v>2.2653721682847898E-2</v>
       </c>
-      <c r="H54" s="31">
-        <f>H36/(H38*4)</f>
+      <c r="H54" s="22">
+        <f t="shared" si="10"/>
         <v>3.4883720930232558E-2</v>
       </c>
-      <c r="I54" s="31">
-        <f>I36/(I38*4)</f>
+      <c r="I54" s="22">
+        <f t="shared" si="10"/>
         <v>0.19359331476323119</v>
       </c>
-      <c r="J54" s="31">
-        <f>J36/(J38*4)</f>
+      <c r="J54" s="22">
+        <f t="shared" si="10"/>
         <v>0.35830999066293184</v>
       </c>
-      <c r="K54" s="34">
-        <f>K36/(K38*4)</f>
+      <c r="K54" s="25">
+        <f t="shared" si="10"/>
         <v>0.78975710617800088</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="B55" s="16">
+      <c r="A55" s="29"/>
+      <c r="B55" s="10">
         <v>8</v>
       </c>
-      <c r="C55" s="17">
-        <f>C36/(C39*8)</f>
+      <c r="C55" s="11">
+        <f t="shared" ref="C55:K55" si="11">C36/(C39*8)</f>
         <v>3.8951841359773369E-3</v>
       </c>
-      <c r="D55" s="17">
-        <f>D36/(D39*8)</f>
+      <c r="D55" s="11">
+        <f t="shared" si="11"/>
         <v>6.3713592233009706E-3</v>
       </c>
-      <c r="E55" s="17">
-        <f>E36/(E39*8)</f>
+      <c r="E55" s="11">
+        <f t="shared" si="11"/>
         <v>7.3394495412844032E-3</v>
       </c>
-      <c r="F55" s="17">
-        <f>F36/(F39*8)</f>
+      <c r="F55" s="11">
+        <f t="shared" si="11"/>
         <v>6.2076749435665919E-3</v>
       </c>
-      <c r="G55" s="17">
-        <f>G36/(G39*8)</f>
+      <c r="G55" s="11">
+        <f t="shared" si="11"/>
         <v>1.0479041916167666E-2</v>
       </c>
-      <c r="H55" s="17">
-        <f>H36/(H39*8)</f>
+      <c r="H55" s="11">
+        <f t="shared" si="11"/>
         <v>8.426966292134833E-3</v>
       </c>
-      <c r="I55" s="17">
-        <f>I36/(I39*8)</f>
+      <c r="I55" s="11">
+        <f t="shared" si="11"/>
         <v>6.5135895032802246E-2</v>
       </c>
-      <c r="J55" s="17">
-        <f>J36/(J39*8)</f>
+      <c r="J55" s="11">
+        <f t="shared" si="11"/>
         <v>0.13455469845722301</v>
       </c>
-      <c r="K55" s="18">
-        <f>K36/(K39*8)</f>
+      <c r="K55" s="12">
+        <f t="shared" si="11"/>
         <v>0.66793497059840878</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A33:J33"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A41:K41"/>
@@ -11055,17 +11102,6 @@
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="C50:K50"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="C34:J34"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="C10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>